<commit_message>
added further wage analysis
</commit_message>
<xml_diff>
--- a/wages.xlsx
+++ b/wages.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Education/spring2024/datascience/cs5830_finalproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA01E20-5448-BB46-AFD7-B0D6E95D0B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683CBA8F-E159-BD42-885B-BAE72042D9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F6F46214-75BB-7840-B11A-50066D2B5C53}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{F6F46214-75BB-7840-B11A-50066D2B5C53}"/>
   </bookViews>
   <sheets>
-    <sheet name="JobTitleAndWage" sheetId="1" r:id="rId1"/>
+    <sheet name="County" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0549BB82-B064-3B47-9DBD-6002917EC574}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>

</xml_diff>